<commit_message>
tabla de métricas v 1.0
</commit_message>
<xml_diff>
--- a/MA/Resolucion/TABME_V1.0_2017.xlsx
+++ b/MA/Resolucion/TABME_V1.0_2017.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB-USR-AQ265-A0805\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7650" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tableros" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,7 @@
     <sheet name="FMEXRI" sheetId="8" r:id="rId4"/>
     <sheet name="FMICIC" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1262,6 +1267,75 @@
     <xf numFmtId="2" fontId="20" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1346,6 +1420,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1370,12 +1450,6 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1403,119 +1477,50 @@
     <xf numFmtId="0" fontId="18" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="18" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="3" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="3" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1586,7 +1591,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1603,9 +1608,12 @@
             <c:strRef>
               <c:f>FMNCONPRO!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>PPQA Numero de N conformidades QA del Producto</c:v>
+                  <c:v>PPQA</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Numero de N conformidades QA del Producto</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1656,7 +1664,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -1669,6 +1677,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1707,10 +1716,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1733,11 +1742,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93630848"/>
-        <c:axId val="93633920"/>
+        <c:axId val="201240384"/>
+        <c:axId val="201241504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93630848"/>
+        <c:axId val="201240384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1813,10 +1822,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93633920"/>
+        <c:crossAx val="201241504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1824,7 +1833,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93633920"/>
+        <c:axId val="201241504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1896,7 +1905,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93630848"/>
+        <c:crossAx val="201240384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1950,7 +1959,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2032,9 +2041,12 @@
             <c:strRef>
               <c:f>FMNCONPRO!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE N CONFORMIDADES QA DE PRODUCTO</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2080,7 +2092,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -2093,6 +2105,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2131,10 +2144,10 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.55000000000000004</c:v>
+                  <c:v>0.83333333333333337</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2155,11 +2168,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="93491968"/>
-        <c:axId val="93493504"/>
+        <c:axId val="201245984"/>
+        <c:axId val="201246544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93491968"/>
+        <c:axId val="201245984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2199,10 +2212,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93493504"/>
+        <c:crossAx val="201246544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2210,7 +2223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93493504"/>
+        <c:axId val="201246544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2231,7 +2244,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93491968"/>
+        <c:crossAx val="201245984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2282,7 +2295,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2338,7 +2351,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2430,11 +2442,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="93583232"/>
-        <c:axId val="100479360"/>
+        <c:axId val="201249344"/>
+        <c:axId val="201249904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="93583232"/>
+        <c:axId val="201249344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2466,7 +2478,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2510,10 +2521,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100479360"/>
+        <c:crossAx val="201249904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2521,7 +2532,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100479360"/>
+        <c:axId val="201249904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2567,7 +2578,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2605,10 +2615,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93583232"/>
+        <c:crossAx val="201249344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2622,7 +2632,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -2651,7 +2660,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2678,7 +2687,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2799,9 +2808,12 @@
             <c:strRef>
               <c:f>FMVREQM!$B$46:$B$47</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE VOLATILIDAD DE REQUERIMIENTOS VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE VOLATILIDAD DE REQUERIMIENTOS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2862,12 +2874,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="100505088"/>
-        <c:axId val="100506624"/>
+        <c:axId val="201252144"/>
+        <c:axId val="201252704"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="100505088"/>
+        <c:axId val="201252144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2901,10 +2913,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100506624"/>
+        <c:crossAx val="201252704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2912,7 +2924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="100506624"/>
+        <c:axId val="201252704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2957,10 +2969,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="100505088"/>
+        <c:crossAx val="201252144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2995,7 +3007,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3111,7 +3123,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3124,6 +3136,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -3188,11 +3201,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101028224"/>
-        <c:axId val="101031296"/>
+        <c:axId val="201255504"/>
+        <c:axId val="261730112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101028224"/>
+        <c:axId val="201255504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3273,10 +3286,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101031296"/>
+        <c:crossAx val="261730112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3284,7 +3297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101031296"/>
+        <c:axId val="261730112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3346,7 +3359,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101028224"/>
+        <c:crossAx val="201255504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3397,7 +3410,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3454,7 +3467,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3569,11 +3581,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="101076992"/>
-        <c:axId val="101078912"/>
+        <c:axId val="261732352"/>
+        <c:axId val="261732912"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="101076992"/>
+        <c:axId val="261732352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3604,7 +3616,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3647,10 +3658,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101078912"/>
+        <c:crossAx val="261732912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3658,7 +3669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101078912"/>
+        <c:axId val="261732912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3703,7 +3714,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3740,10 +3750,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101076992"/>
+        <c:crossAx val="261732352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3794,7 +3804,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3853,7 +3863,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-ES"/>
+          <a:endParaRPr lang="es-PE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3870,9 +3880,12 @@
             <c:strRef>
               <c:f>FMICIC!$B$31:$C$31</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>CM Numero de Items Modificados</c:v>
+                  <c:v>CM</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Numero de Items Modificados</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3923,7 +3936,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -4000,11 +4013,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="101173120"/>
-        <c:axId val="101176448"/>
+        <c:axId val="261735712"/>
+        <c:axId val="261736272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="101173120"/>
+        <c:axId val="261735712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4036,7 +4049,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4080,10 +4092,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="101176448"/>
+        <c:crossAx val="261736272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4091,7 +4103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="101176448"/>
+        <c:axId val="261736272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4154,7 +4166,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4168,7 +4179,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="101173120"/>
+        <c:crossAx val="261735712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4222,7 +4233,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4304,9 +4315,12 @@
             <c:strRef>
               <c:f>FMICIC!$C$39:$C$40</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>TABLERO DE METRICAS DE INDICE DE CAMBIOS DE ITEMS DE CONFIGURACION VALORES</c:v>
+                  <c:v>TABLERO DE METRICAS DE INDICE DE CAMBIOS DE ITEMS DE CONFIGURACION</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>VALORES</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4352,7 +4366,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="es-ES"/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="inEnd"/>
@@ -4427,11 +4441,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="93614464"/>
-        <c:axId val="93616000"/>
+        <c:axId val="261738512"/>
+        <c:axId val="261739072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="93614464"/>
+        <c:axId val="261738512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4471,10 +4485,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-ES"/>
+            <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="93616000"/>
+        <c:crossAx val="261739072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4482,7 +4496,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93616000"/>
+        <c:axId val="261739072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4503,7 +4517,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="93614464"/>
+        <c:crossAx val="261738512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4554,7 +4568,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-ES"/>
+      <a:endParaRPr lang="es-PE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5431,7 +5445,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5457,152 +5471,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" customHeight="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="87"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="109"/>
+      <c r="N1" s="109"/>
+      <c r="O1" s="109"/>
+      <c r="P1" s="110"/>
     </row>
     <row r="2" spans="1:16" ht="15" customHeight="1">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="89"/>
-      <c r="N2" s="89"/>
-      <c r="O2" s="89"/>
-      <c r="P2" s="90"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="112"/>
+      <c r="N2" s="112"/>
+      <c r="O2" s="112"/>
+      <c r="P2" s="113"/>
     </row>
     <row r="3" spans="1:16" ht="15" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="90"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="113"/>
     </row>
     <row r="4" spans="1:16" ht="15" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="89"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="90"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="112"/>
+      <c r="N4" s="112"/>
+      <c r="O4" s="112"/>
+      <c r="P4" s="113"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="90"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="112"/>
+      <c r="N5" s="112"/>
+      <c r="O5" s="112"/>
+      <c r="P5" s="113"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="92"/>
-      <c r="O6" s="92"/>
-      <c r="P6" s="93"/>
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="115"/>
+      <c r="N6" s="115"/>
+      <c r="O6" s="115"/>
+      <c r="P6" s="116"/>
     </row>
     <row r="7" spans="1:16" ht="15" customHeight="1">
-      <c r="A7" s="94" t="s">
+      <c r="A7" s="117" t="s">
         <v>63</v>
       </c>
-      <c r="B7" s="95"/>
-      <c r="C7" s="95"/>
-      <c r="D7" s="95"/>
-      <c r="E7" s="95"/>
-      <c r="F7" s="95"/>
-      <c r="G7" s="95"/>
-      <c r="H7" s="95"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="95"/>
-      <c r="K7" s="95"/>
-      <c r="L7" s="95"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="95"/>
-      <c r="O7" s="95"/>
-      <c r="P7" s="96"/>
+      <c r="B7" s="118"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
+      <c r="G7" s="118"/>
+      <c r="H7" s="118"/>
+      <c r="I7" s="118"/>
+      <c r="J7" s="118"/>
+      <c r="K7" s="118"/>
+      <c r="L7" s="118"/>
+      <c r="M7" s="118"/>
+      <c r="N7" s="118"/>
+      <c r="O7" s="118"/>
+      <c r="P7" s="119"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="97"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="98"/>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
-      <c r="G8" s="98"/>
-      <c r="H8" s="98"/>
-      <c r="I8" s="98"/>
-      <c r="J8" s="98"/>
-      <c r="K8" s="98"/>
-      <c r="L8" s="98"/>
-      <c r="M8" s="98"/>
-      <c r="N8" s="98"/>
-      <c r="O8" s="98"/>
-      <c r="P8" s="99"/>
+      <c r="A8" s="120"/>
+      <c r="B8" s="121"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="121"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="121"/>
+      <c r="G8" s="121"/>
+      <c r="H8" s="121"/>
+      <c r="I8" s="121"/>
+      <c r="J8" s="121"/>
+      <c r="K8" s="121"/>
+      <c r="L8" s="121"/>
+      <c r="M8" s="121"/>
+      <c r="N8" s="121"/>
+      <c r="O8" s="121"/>
+      <c r="P8" s="122"/>
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1">
       <c r="A9" s="19"/>
@@ -5619,48 +5633,48 @@
       <c r="A10" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="105"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="106"/>
+      <c r="C10" s="128"/>
+      <c r="D10" s="128"/>
+      <c r="E10" s="128"/>
+      <c r="F10" s="128"/>
+      <c r="G10" s="128"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="129"/>
     </row>
     <row r="11" spans="1:16" ht="16.5" thickBot="1">
-      <c r="A11" s="107" t="s">
+      <c r="A11" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="108"/>
-      <c r="C11" s="108"/>
-      <c r="D11" s="108"/>
-      <c r="E11" s="108"/>
-      <c r="F11" s="108"/>
-      <c r="G11" s="108"/>
-      <c r="H11" s="108"/>
-      <c r="I11" s="109"/>
+      <c r="B11" s="131"/>
+      <c r="C11" s="131"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="131"/>
+      <c r="F11" s="131"/>
+      <c r="G11" s="131"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="132"/>
     </row>
     <row r="12" spans="1:16" ht="15.75" thickBot="1">
       <c r="A12" s="70"/>
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="100" t="s">
+      <c r="C12" s="124"/>
+      <c r="D12" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="102"/>
-      <c r="F12" s="103" t="s">
+      <c r="E12" s="125"/>
+      <c r="F12" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="G12" s="102"/>
-      <c r="H12" s="103" t="s">
+      <c r="G12" s="125"/>
+      <c r="H12" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="102"/>
+      <c r="I12" s="125"/>
     </row>
     <row r="13" spans="1:16" ht="26.25" thickBot="1">
       <c r="A13" s="1" t="s">
@@ -5790,15 +5804,15 @@
       <c r="I17" s="16"/>
     </row>
     <row r="18" spans="1:16" ht="19.5" thickBot="1">
-      <c r="J18" s="82" t="s">
+      <c r="J18" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="K18" s="83"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="83"/>
-      <c r="N18" s="83"/>
-      <c r="O18" s="83"/>
-      <c r="P18" s="84"/>
+      <c r="K18" s="106"/>
+      <c r="L18" s="106"/>
+      <c r="M18" s="106"/>
+      <c r="N18" s="106"/>
+      <c r="O18" s="106"/>
+      <c r="P18" s="107"/>
     </row>
     <row r="19" spans="1:16" ht="32.25" customHeight="1">
       <c r="J19" s="17" t="s">
@@ -5832,11 +5846,11 @@
       </c>
       <c r="L20" s="75">
         <f>FMNCONPRO!D33</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="M20" s="75">
         <f>FMNCONPRO!E33</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="N20" s="75" t="e">
         <f>FMNCONPRO!#REF!</f>
@@ -5848,7 +5862,7 @@
       </c>
       <c r="P20" s="75">
         <f>FMNCONPRO!G33</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="30" customHeight="1">
@@ -6048,8 +6062,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6067,20 +6081,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="87"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
       <c r="M1" s="33"/>
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
@@ -6089,18 +6103,18 @@
       <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="113"/>
       <c r="M2" s="33"/>
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
@@ -6109,18 +6123,18 @@
       <c r="R2" s="33"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="113"/>
       <c r="M3" s="33"/>
       <c r="N3" s="33"/>
       <c r="O3" s="33"/>
@@ -6129,18 +6143,18 @@
       <c r="R3" s="33"/>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="90"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="113"/>
       <c r="M4" s="33"/>
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
@@ -6149,18 +6163,18 @@
       <c r="R4" s="33"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
       <c r="M5" s="33"/>
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
@@ -6169,18 +6183,18 @@
       <c r="R5" s="33"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="93"/>
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="116"/>
       <c r="M6" s="33"/>
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
@@ -6190,16 +6204,16 @@
     </row>
     <row r="7" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:18">
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="135" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="111"/>
-      <c r="E8" s="112"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
     </row>
     <row r="9" spans="1:18" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C9" s="113"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="115"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="140"/>
     </row>
     <row r="10" spans="1:18" ht="26.25" thickBot="1">
       <c r="C10" s="2" t="s">
@@ -6247,16 +6261,16 @@
     </row>
     <row r="14" spans="1:18" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:18" ht="32.25" customHeight="1" thickBot="1">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="119"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47"/>
     </row>
@@ -6300,32 +6314,32 @@
         <v>67</v>
       </c>
       <c r="E17" s="44">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F17" s="44">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G17" s="45">
         <f>E17/F17</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H17" s="46">
         <f>+G17</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="20" spans="1:10" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A20" s="118" t="s">
+      <c r="A20" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="119"/>
-      <c r="C20" s="119"/>
-      <c r="D20" s="119"/>
-      <c r="E20" s="119"/>
-      <c r="F20" s="119"/>
-      <c r="G20" s="119"/>
-      <c r="H20" s="119"/>
+      <c r="B20" s="134"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
+      <c r="F20" s="134"/>
+      <c r="G20" s="134"/>
+      <c r="H20" s="134"/>
     </row>
     <row r="21" spans="1:10" ht="36.75" thickBot="1">
       <c r="A21" s="36" t="s">
@@ -6367,18 +6381,18 @@
         <v>68</v>
       </c>
       <c r="E22" s="44">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F22" s="44">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="G22" s="45">
         <f>E22/F22</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="H22" s="46">
         <f>+G22</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="33.75" customHeight="1">
@@ -6392,14 +6406,14 @@
       <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:10" ht="30.75" customHeight="1">
-      <c r="A24" s="132"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="132"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="152"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="152"/>
+      <c r="F24" s="152"/>
+      <c r="G24" s="152"/>
+      <c r="H24" s="152"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="49"/>
@@ -6412,14 +6426,14 @@
       <c r="H25" s="49"/>
     </row>
     <row r="26" spans="1:10" ht="21">
-      <c r="A26" s="133"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="135"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="49"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="137"/>
-      <c r="H26" s="137"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
     </row>
     <row r="27" spans="1:10" ht="21">
       <c r="A27" s="50"/>
@@ -6433,16 +6447,16 @@
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="29" spans="1:10" ht="42.75" customHeight="1" thickBot="1">
-      <c r="A29" s="118" t="s">
+      <c r="A29" s="133" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="119"/>
-      <c r="C29" s="119"/>
-      <c r="D29" s="119"/>
-      <c r="E29" s="119"/>
-      <c r="F29" s="119"/>
-      <c r="G29" s="119"/>
-      <c r="H29" s="148"/>
+      <c r="B29" s="134"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="134"/>
+      <c r="E29" s="134"/>
+      <c r="F29" s="134"/>
+      <c r="G29" s="134"/>
+      <c r="H29" s="94"/>
       <c r="I29" s="47"/>
       <c r="J29" s="47"/>
     </row>
@@ -6459,11 +6473,11 @@
       <c r="D30" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="146" t="s">
+      <c r="E30" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="125"/>
-      <c r="G30" s="126"/>
+      <c r="F30" s="148"/>
+      <c r="G30" s="149"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
     </row>
@@ -6478,27 +6492,27 @@
         <v>7</v>
       </c>
       <c r="D31" s="13">
-        <v>22</v>
-      </c>
-      <c r="E31" s="147">
-        <v>22</v>
-      </c>
-      <c r="F31" s="127"/>
-      <c r="G31" s="128"/>
+        <v>20</v>
+      </c>
+      <c r="E31" s="93">
+        <v>20</v>
+      </c>
+      <c r="F31" s="150"/>
+      <c r="G31" s="151"/>
       <c r="H31" s="50"/>
       <c r="I31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="24">
-      <c r="A32" s="120" t="s">
+      <c r="A32" s="143" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="121"/>
-      <c r="C32" s="121"/>
+      <c r="B32" s="144"/>
+      <c r="C32" s="144"/>
       <c r="D32" s="20">
-        <v>40</v>
-      </c>
-      <c r="E32" s="139">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="E32" s="89">
+        <v>24</v>
       </c>
       <c r="F32" s="53" t="s">
         <v>36</v>
@@ -6508,18 +6522,18 @@
       </c>
     </row>
     <row r="33" spans="1:20" ht="27" thickBot="1">
-      <c r="A33" s="122" t="s">
+      <c r="A33" s="145" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="123"/>
-      <c r="C33" s="124"/>
+      <c r="B33" s="146"/>
+      <c r="C33" s="147"/>
       <c r="D33" s="57">
         <f>D31/D32</f>
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="E33" s="145">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E33" s="91">
         <f>E31/E32</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="F33" s="58">
         <f>+I33</f>
@@ -6527,7 +6541,7 @@
       </c>
       <c r="G33" s="59">
         <f>AVERAGE(D33:E33)</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="34" spans="1:20">
@@ -6535,10 +6549,10 @@
     </row>
     <row r="38" spans="1:20" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:20" ht="39.75" customHeight="1">
-      <c r="B39" s="116" t="s">
+      <c r="B39" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="C39" s="117"/>
+      <c r="C39" s="142"/>
       <c r="D39" s="21"/>
       <c r="E39" s="21"/>
       <c r="F39" s="21"/>
@@ -6562,7 +6576,7 @@
       </c>
       <c r="C41" s="35">
         <f>D33</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
     <row r="42" spans="1:20">
@@ -6571,7 +6585,7 @@
       </c>
       <c r="C42" s="35">
         <f>E31/E32</f>
-        <v>0.55000000000000004</v>
+        <v>0.83333333333333337</v>
       </c>
     </row>
   </sheetData>
@@ -6720,103 +6734,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="87"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="110"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="90"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="113"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="90"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="113"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="90"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="113"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="113"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="93"/>
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="116"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:12">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="135" t="s">
         <v>60</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="112"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="137"/>
     </row>
     <row r="9" spans="1:12" ht="33" customHeight="1" thickBot="1">
-      <c r="A9" s="113"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="140"/>
     </row>
     <row r="10" spans="1:12" ht="26.25" thickBot="1">
       <c r="A10" s="2" t="s">
@@ -6864,18 +6878,18 @@
     </row>
     <row r="14" spans="1:12" ht="15.75" thickBot="1"/>
     <row r="15" spans="1:12" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="119"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
-      <c r="F15" s="119"/>
-      <c r="G15" s="119"/>
-      <c r="H15" s="119"/>
-      <c r="I15" s="150"/>
-      <c r="J15" s="149"/>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="134"/>
+      <c r="H15" s="134"/>
+      <c r="I15" s="153"/>
+      <c r="J15" s="95"/>
     </row>
     <row r="16" spans="1:12" ht="30.75" customHeight="1" thickBot="1">
       <c r="A16" s="29" t="s">
@@ -6919,7 +6933,7 @@
       <c r="D17" s="26">
         <v>0</v>
       </c>
-      <c r="E17" s="151">
+      <c r="E17" s="96">
         <v>0</v>
       </c>
       <c r="F17" s="26">
@@ -6941,16 +6955,16 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="21" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A21" s="118" t="s">
+      <c r="A21" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="119"/>
-      <c r="C21" s="119"/>
-      <c r="D21" s="119"/>
-      <c r="E21" s="119"/>
-      <c r="F21" s="119"/>
-      <c r="G21" s="119"/>
-      <c r="H21" s="119"/>
+      <c r="B21" s="134"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
+      <c r="F21" s="134"/>
+      <c r="G21" s="134"/>
+      <c r="H21" s="134"/>
     </row>
     <row r="22" spans="1:9" ht="36.75" thickBot="1">
       <c r="A22" s="36" t="s">
@@ -7008,16 +7022,16 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" thickBot="1"/>
     <row r="27" spans="1:9" ht="19.5" thickBot="1">
-      <c r="A27" s="118" t="s">
+      <c r="A27" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="119"/>
+      <c r="B27" s="134"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
+      <c r="G27" s="134"/>
+      <c r="H27" s="134"/>
     </row>
     <row r="28" spans="1:9" ht="36.75" thickBot="1">
       <c r="A28" s="36" t="s">
@@ -7084,14 +7098,14 @@
       <c r="H30" s="74"/>
     </row>
     <row r="31" spans="1:9" ht="18.75">
-      <c r="A31" s="130"/>
-      <c r="B31" s="130"/>
-      <c r="C31" s="130"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
+      <c r="A31" s="156"/>
+      <c r="B31" s="156"/>
+      <c r="C31" s="156"/>
+      <c r="D31" s="156"/>
+      <c r="E31" s="156"/>
+      <c r="F31" s="156"/>
+      <c r="G31" s="156"/>
+      <c r="H31" s="156"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="49"/>
@@ -7107,7 +7121,7 @@
       <c r="A33" s="50"/>
       <c r="B33" s="71"/>
       <c r="C33" s="77"/>
-      <c r="D33" s="131"/>
+      <c r="D33" s="82"/>
       <c r="E33" s="73"/>
       <c r="F33" s="73"/>
       <c r="G33" s="78"/>
@@ -7115,16 +7129,16 @@
     </row>
     <row r="38" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="39" spans="1:8" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A39" s="118" t="s">
+      <c r="A39" s="133" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="119"/>
-      <c r="C39" s="119"/>
-      <c r="D39" s="119"/>
-      <c r="E39" s="119"/>
-      <c r="F39" s="119"/>
-      <c r="G39" s="150"/>
-      <c r="H39" s="149"/>
+      <c r="B39" s="134"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="134"/>
+      <c r="G39" s="153"/>
+      <c r="H39" s="95"/>
     </row>
     <row r="40" spans="1:8" ht="24.75" thickBot="1">
       <c r="A40" s="52" t="s">
@@ -7142,8 +7156,8 @@
       <c r="E40" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="F40" s="125"/>
-      <c r="G40" s="126"/>
+      <c r="F40" s="148"/>
+      <c r="G40" s="149"/>
     </row>
     <row r="41" spans="1:8" ht="54" customHeight="1" thickBot="1">
       <c r="A41" s="55" t="s">
@@ -7158,22 +7172,22 @@
       <c r="D41" s="13">
         <v>0</v>
       </c>
-      <c r="E41" s="144">
+      <c r="E41" s="90">
         <v>0</v>
       </c>
-      <c r="F41" s="127"/>
-      <c r="G41" s="128"/>
+      <c r="F41" s="150"/>
+      <c r="G41" s="151"/>
     </row>
     <row r="42" spans="1:8" ht="24">
-      <c r="A42" s="120" t="s">
+      <c r="A42" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="121"/>
-      <c r="C42" s="121"/>
+      <c r="B42" s="144"/>
+      <c r="C42" s="144"/>
       <c r="D42" s="20">
         <v>13</v>
       </c>
-      <c r="E42" s="139">
+      <c r="E42" s="89">
         <v>13</v>
       </c>
       <c r="F42" s="53" t="s">
@@ -7184,16 +7198,16 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="27" thickBot="1">
-      <c r="A43" s="122" t="s">
+      <c r="A43" s="145" t="s">
         <v>43</v>
       </c>
-      <c r="B43" s="123"/>
-      <c r="C43" s="124"/>
+      <c r="B43" s="146"/>
+      <c r="C43" s="147"/>
       <c r="D43" s="57">
         <f>D41/D42*100</f>
         <v>0</v>
       </c>
-      <c r="E43" s="145">
+      <c r="E43" s="91">
         <f>E41/E42*100</f>
         <v>0</v>
       </c>
@@ -7208,10 +7222,10 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="46" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A46" s="165" t="s">
+      <c r="A46" s="154" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="166"/>
+      <c r="B46" s="155"/>
     </row>
     <row r="47" spans="1:8" ht="15.75">
       <c r="A47" s="22" t="s">
@@ -7241,17 +7255,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A15:I15"/>
-    <mergeCell ref="F40:G41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
     <mergeCell ref="A46:B46"/>
     <mergeCell ref="A31:H31"/>
     <mergeCell ref="A1:L6"/>
     <mergeCell ref="A8:C9"/>
     <mergeCell ref="A21:H21"/>
     <mergeCell ref="A27:H27"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A15:I15"/>
+    <mergeCell ref="F40:G41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -7383,7 +7397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
@@ -7393,91 +7407,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="87"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="110"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="90"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="113"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="90"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="113"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="90"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="113"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="90"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="113"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="93"/>
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="116"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:10">
-      <c r="A8" s="110" t="s">
+      <c r="A8" s="135" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="111"/>
-      <c r="C8" s="112"/>
+      <c r="B8" s="136"/>
+      <c r="C8" s="137"/>
     </row>
     <row r="9" spans="1:10" ht="33" customHeight="1" thickBot="1">
-      <c r="A9" s="113"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="138"/>
+      <c r="B9" s="139"/>
+      <c r="C9" s="140"/>
     </row>
     <row r="10" spans="1:10" ht="26.25" thickBot="1">
       <c r="A10" s="1" t="s">
@@ -7524,15 +7538,15 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="140" t="s">
+      <c r="A15" s="157" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="141"/>
-      <c r="C15" s="141"/>
-      <c r="D15" s="141"/>
-      <c r="E15" s="141"/>
-      <c r="F15" s="141"/>
-      <c r="G15" s="141"/>
+      <c r="B15" s="158"/>
+      <c r="C15" s="158"/>
+      <c r="D15" s="158"/>
+      <c r="E15" s="158"/>
+      <c r="F15" s="158"/>
+      <c r="G15" s="158"/>
     </row>
     <row r="16" spans="1:10" ht="36.75" thickBot="1">
       <c r="A16" s="36" t="s">
@@ -7573,25 +7587,25 @@
       <c r="E17" s="62">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F17" s="157">
+      <c r="F17" s="99">
         <f>E17/4.5</f>
         <v>0.25777777777777777</v>
       </c>
-      <c r="G17" s="158">
+      <c r="G17" s="100">
         <f>+F17</f>
         <v>0.25777777777777777</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A22" s="142" t="s">
+      <c r="A22" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="143"/>
-      <c r="C22" s="143"/>
-      <c r="D22" s="143"/>
-      <c r="E22" s="143"/>
-      <c r="F22" s="143"/>
-      <c r="G22" s="143"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="161"/>
+      <c r="D22" s="161"/>
+      <c r="E22" s="161"/>
+      <c r="F22" s="161"/>
+      <c r="G22" s="161"/>
     </row>
     <row r="23" spans="1:7" ht="36.75" thickBot="1">
       <c r="A23" s="36" t="s">
@@ -7632,22 +7646,22 @@
       <c r="E24" s="62">
         <v>1.1599999999999999</v>
       </c>
-      <c r="F24" s="163">
+      <c r="F24" s="104">
         <f>E24/4.5</f>
         <v>0.25777777777777777</v>
       </c>
-      <c r="G24" s="162">
+      <c r="G24" s="103">
         <f>+F24</f>
         <v>0.25777777777777777</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75">
-      <c r="A27" s="132"/>
-      <c r="B27" s="132"/>
-      <c r="C27" s="132"/>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
+      <c r="A27" s="152"/>
+      <c r="B27" s="152"/>
+      <c r="C27" s="152"/>
+      <c r="D27" s="152"/>
+      <c r="E27" s="152"/>
+      <c r="F27" s="152"/>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" s="49"/>
@@ -7658,46 +7672,46 @@
       <c r="F28" s="49"/>
     </row>
     <row r="29" spans="1:7" ht="21">
-      <c r="A29" s="133"/>
-      <c r="B29" s="134"/>
-      <c r="C29" s="138"/>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="136"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="84"/>
+      <c r="C29" s="88"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="86"/>
     </row>
     <row r="34" spans="1:14" ht="19.5" customHeight="1">
-      <c r="A34" s="153" t="s">
+      <c r="A34" s="159" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="153"/>
-      <c r="C34" s="153"/>
-      <c r="D34" s="153"/>
-      <c r="E34" s="153"/>
-      <c r="F34" s="153"/>
-      <c r="G34" s="153"/>
-      <c r="H34" s="149"/>
+      <c r="B34" s="159"/>
+      <c r="C34" s="159"/>
+      <c r="D34" s="159"/>
+      <c r="E34" s="159"/>
+      <c r="F34" s="159"/>
+      <c r="G34" s="159"/>
+      <c r="H34" s="95"/>
       <c r="L34" s="64"/>
       <c r="M34" s="65"/>
       <c r="N34" s="65"/>
     </row>
     <row r="35" spans="1:14" ht="24">
-      <c r="A35" s="152" t="s">
+      <c r="A35" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="152" t="s">
+      <c r="B35" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="152" t="s">
+      <c r="C35" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="152" t="s">
+      <c r="D35" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="152" t="s">
+      <c r="E35" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="154"/>
-      <c r="G35" s="154"/>
+      <c r="F35" s="164"/>
+      <c r="G35" s="164"/>
       <c r="K35" s="64"/>
       <c r="L35" s="65"/>
       <c r="M35" s="65"/>
@@ -7709,7 +7723,7 @@
       <c r="B36" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="159" t="s">
+      <c r="C36" s="101" t="s">
         <v>10</v>
       </c>
       <c r="D36" s="80">
@@ -7718,52 +7732,52 @@
       <c r="E36" s="80">
         <v>26</v>
       </c>
-      <c r="F36" s="154"/>
-      <c r="G36" s="154"/>
+      <c r="F36" s="164"/>
+      <c r="G36" s="164"/>
       <c r="K36" s="64"/>
       <c r="L36" s="65"/>
       <c r="M36" s="65"/>
     </row>
     <row r="37" spans="1:14" ht="26.25" customHeight="1">
-      <c r="A37" s="160" t="s">
+      <c r="A37" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="160"/>
-      <c r="C37" s="160"/>
-      <c r="D37" s="164">
+      <c r="B37" s="162"/>
+      <c r="C37" s="162"/>
+      <c r="D37" s="163">
         <v>26</v>
       </c>
-      <c r="E37" s="164">
+      <c r="E37" s="163">
         <v>26</v>
       </c>
-      <c r="F37" s="152" t="s">
+      <c r="F37" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="G37" s="152" t="s">
+      <c r="G37" s="97" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="160"/>
-      <c r="B38" s="160"/>
-      <c r="C38" s="160"/>
-      <c r="D38" s="164"/>
-      <c r="E38" s="164"/>
+      <c r="A38" s="162"/>
+      <c r="B38" s="162"/>
+      <c r="C38" s="162"/>
+      <c r="D38" s="163"/>
+      <c r="E38" s="163"/>
       <c r="F38" s="63">
         <f>+G38</f>
         <v>26</v>
       </c>
-      <c r="G38" s="161">
+      <c r="G38" s="102">
         <f>AVERAGE(D37:E37)</f>
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="15.75" thickBot="1"/>
     <row r="43" spans="1:14" ht="18.75">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="141" t="s">
         <v>26</v>
       </c>
-      <c r="B43" s="117"/>
+      <c r="B43" s="142"/>
     </row>
     <row r="44" spans="1:14" ht="15.75">
       <c r="A44" s="22" t="s">
@@ -7791,17 +7805,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A1:J6"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="F35:G36"/>
+    <mergeCell ref="A27:F27"/>
     <mergeCell ref="A15:G15"/>
     <mergeCell ref="A34:G34"/>
     <mergeCell ref="A22:G22"/>
     <mergeCell ref="A37:C38"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="E37:E38"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A1:J6"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="F35:G36"/>
-    <mergeCell ref="A27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7914,21 +7928,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="108" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="87"/>
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+      <c r="H1" s="109"/>
+      <c r="I1" s="109"/>
+      <c r="J1" s="109"/>
+      <c r="K1" s="109"/>
+      <c r="L1" s="109"/>
+      <c r="M1" s="110"/>
       <c r="N1" s="33"/>
       <c r="O1" s="33"/>
       <c r="P1" s="33"/>
@@ -7937,19 +7951,19 @@
       <c r="S1" s="33"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="88"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
-      <c r="J2" s="89"/>
-      <c r="K2" s="89"/>
-      <c r="L2" s="89"/>
-      <c r="M2" s="90"/>
+      <c r="A2" s="111"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
+      <c r="M2" s="113"/>
       <c r="N2" s="33"/>
       <c r="O2" s="33"/>
       <c r="P2" s="33"/>
@@ -7958,19 +7972,19 @@
       <c r="S2" s="33"/>
     </row>
     <row r="3" spans="1:19" ht="15" customHeight="1">
-      <c r="A3" s="88"/>
-      <c r="B3" s="89"/>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
+      <c r="A3" s="111"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="113"/>
       <c r="N3" s="33"/>
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
@@ -7979,19 +7993,19 @@
       <c r="S3" s="33"/>
     </row>
     <row r="4" spans="1:19" ht="15" customHeight="1">
-      <c r="A4" s="88"/>
-      <c r="B4" s="89"/>
-      <c r="C4" s="89"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="89"/>
-      <c r="F4" s="89"/>
-      <c r="G4" s="89"/>
-      <c r="H4" s="89"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="89"/>
-      <c r="K4" s="89"/>
-      <c r="L4" s="89"/>
-      <c r="M4" s="90"/>
+      <c r="A4" s="111"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="112"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="112"/>
+      <c r="F4" s="112"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="112"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="112"/>
+      <c r="K4" s="112"/>
+      <c r="L4" s="112"/>
+      <c r="M4" s="113"/>
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
       <c r="P4" s="33"/>
@@ -8000,19 +8014,19 @@
       <c r="S4" s="33"/>
     </row>
     <row r="5" spans="1:19" ht="15.75" customHeight="1">
-      <c r="A5" s="88"/>
-      <c r="B5" s="89"/>
-      <c r="C5" s="89"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="89"/>
-      <c r="G5" s="89"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="89"/>
-      <c r="M5" s="90"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="112"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="112"/>
+      <c r="F5" s="112"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="112"/>
+      <c r="I5" s="112"/>
+      <c r="J5" s="112"/>
+      <c r="K5" s="112"/>
+      <c r="L5" s="112"/>
+      <c r="M5" s="113"/>
       <c r="N5" s="33"/>
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
@@ -8021,19 +8035,19 @@
       <c r="S5" s="33"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="91"/>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
-      <c r="J6" s="92"/>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="93"/>
+      <c r="A6" s="114"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
+      <c r="F6" s="115"/>
+      <c r="G6" s="115"/>
+      <c r="H6" s="115"/>
+      <c r="I6" s="115"/>
+      <c r="J6" s="115"/>
+      <c r="K6" s="115"/>
+      <c r="L6" s="115"/>
+      <c r="M6" s="116"/>
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
       <c r="P6" s="33"/>
@@ -8043,16 +8057,16 @@
     </row>
     <row r="7" spans="1:19" ht="15.75" thickBot="1"/>
     <row r="8" spans="1:19">
-      <c r="C8" s="110" t="s">
+      <c r="C8" s="135" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="111"/>
-      <c r="E8" s="112"/>
+      <c r="D8" s="136"/>
+      <c r="E8" s="137"/>
     </row>
     <row r="9" spans="1:19" ht="23.25" customHeight="1" thickBot="1">
-      <c r="C9" s="113"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="115"/>
+      <c r="C9" s="138"/>
+      <c r="D9" s="139"/>
+      <c r="E9" s="140"/>
     </row>
     <row r="10" spans="1:19" ht="26.25" thickBot="1">
       <c r="C10" s="2" t="s">
@@ -8099,43 +8113,43 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="32.25" customHeight="1">
-      <c r="A15" s="153" t="s">
+      <c r="A15" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="153"/>
-      <c r="C15" s="153"/>
-      <c r="D15" s="153"/>
-      <c r="E15" s="153"/>
-      <c r="F15" s="153"/>
-      <c r="G15" s="153"/>
-      <c r="H15" s="153"/>
-      <c r="I15" s="149"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
+      <c r="H15" s="159"/>
+      <c r="I15" s="95"/>
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
     </row>
     <row r="16" spans="1:19" ht="36">
-      <c r="A16" s="152" t="s">
+      <c r="A16" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="152" t="s">
+      <c r="B16" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="152" t="s">
+      <c r="C16" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="152" t="s">
+      <c r="D16" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="152" t="s">
+      <c r="E16" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="F16" s="152" t="s">
+      <c r="F16" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="G16" s="152" t="s">
+      <c r="G16" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="152" t="s">
+      <c r="H16" s="97" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8168,41 +8182,41 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A20" s="153" t="s">
+      <c r="A20" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="153"/>
-      <c r="C20" s="153"/>
-      <c r="D20" s="153"/>
-      <c r="E20" s="153"/>
-      <c r="F20" s="153"/>
-      <c r="G20" s="153"/>
-      <c r="H20" s="153"/>
-      <c r="I20" s="149"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="159"/>
+      <c r="D20" s="159"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="159"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="159"/>
+      <c r="I20" s="95"/>
     </row>
     <row r="21" spans="1:11" ht="48.75" customHeight="1">
-      <c r="A21" s="152" t="s">
+      <c r="A21" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="152" t="s">
+      <c r="B21" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="152" t="s">
+      <c r="C21" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="152" t="s">
+      <c r="D21" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="152" t="s">
+      <c r="E21" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="152" t="s">
+      <c r="F21" s="97" t="s">
         <v>53</v>
       </c>
-      <c r="G21" s="152" t="s">
+      <c r="G21" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="H21" s="152" t="s">
+      <c r="H21" s="97" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8246,15 +8260,15 @@
       <c r="I23" s="74"/>
     </row>
     <row r="24" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A24" s="132"/>
-      <c r="B24" s="132"/>
-      <c r="C24" s="132"/>
-      <c r="D24" s="132"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="132"/>
-      <c r="H24" s="132"/>
-      <c r="I24" s="132"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="152"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="152"/>
+      <c r="F24" s="152"/>
+      <c r="G24" s="152"/>
+      <c r="H24" s="152"/>
+      <c r="I24" s="152"/>
     </row>
     <row r="25" spans="1:11" ht="48.75" customHeight="1">
       <c r="A25" s="49"/>
@@ -8268,15 +8282,15 @@
       <c r="I25" s="49"/>
     </row>
     <row r="26" spans="1:11" ht="21">
-      <c r="A26" s="133"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="135"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="136"/>
-      <c r="F26" s="136"/>
-      <c r="G26" s="136"/>
-      <c r="H26" s="137"/>
-      <c r="I26" s="137"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="84"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
     </row>
     <row r="27" spans="1:11" ht="21">
       <c r="A27" s="50"/>
@@ -8290,38 +8304,38 @@
       <c r="I27" s="74"/>
     </row>
     <row r="29" spans="1:11" ht="42.75" customHeight="1">
-      <c r="A29" s="153" t="s">
+      <c r="A29" s="159" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="153"/>
-      <c r="C29" s="153"/>
-      <c r="D29" s="153"/>
-      <c r="E29" s="153"/>
-      <c r="F29" s="153"/>
-      <c r="G29" s="153"/>
-      <c r="H29" s="149"/>
-      <c r="I29" s="149"/>
+      <c r="B29" s="159"/>
+      <c r="C29" s="159"/>
+      <c r="D29" s="159"/>
+      <c r="E29" s="159"/>
+      <c r="F29" s="159"/>
+      <c r="G29" s="159"/>
+      <c r="H29" s="95"/>
+      <c r="I29" s="95"/>
       <c r="J29" s="47"/>
       <c r="K29" s="47"/>
     </row>
     <row r="30" spans="1:11" s="32" customFormat="1" ht="45.75" customHeight="1">
-      <c r="A30" s="152" t="s">
+      <c r="A30" s="97" t="s">
         <v>32</v>
       </c>
-      <c r="B30" s="152" t="s">
+      <c r="B30" s="97" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="152" t="s">
+      <c r="C30" s="97" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="152" t="s">
+      <c r="D30" s="97" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="152" t="s">
+      <c r="E30" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="154"/>
-      <c r="G30" s="154"/>
+      <c r="F30" s="164"/>
+      <c r="G30" s="164"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
     </row>
@@ -8341,41 +8355,41 @@
       <c r="E31" s="79">
         <v>0</v>
       </c>
-      <c r="F31" s="154"/>
-      <c r="G31" s="154"/>
+      <c r="F31" s="164"/>
+      <c r="G31" s="164"/>
       <c r="H31" s="50"/>
       <c r="I31" s="51"/>
     </row>
     <row r="32" spans="1:11" ht="28.5" customHeight="1">
-      <c r="A32" s="129" t="s">
+      <c r="A32" s="165" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="129"/>
-      <c r="C32" s="129"/>
+      <c r="B32" s="165"/>
+      <c r="C32" s="165"/>
       <c r="D32" s="79">
         <v>22</v>
       </c>
       <c r="E32" s="79">
         <v>22</v>
       </c>
-      <c r="F32" s="152" t="s">
+      <c r="F32" s="97" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="152" t="s">
+      <c r="G32" s="97" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:21" ht="26.25">
-      <c r="A33" s="155" t="s">
+      <c r="A33" s="166" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="155"/>
-      <c r="C33" s="155"/>
-      <c r="D33" s="156">
+      <c r="B33" s="166"/>
+      <c r="C33" s="166"/>
+      <c r="D33" s="98">
         <f>D31/D32</f>
         <v>0</v>
       </c>
-      <c r="E33" s="156">
+      <c r="E33" s="98">
         <f>E31/E32</f>
         <v>0</v>
       </c>
@@ -8383,7 +8397,7 @@
         <f>+I33</f>
         <v>0</v>
       </c>
-      <c r="G33" s="156">
+      <c r="G33" s="98">
         <f>AVERAGE(D33:E33)</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
tabla metrica version final
</commit_message>
<xml_diff>
--- a/MA/Resolucion/TABME_V1.0_2017.xlsx
+++ b/MA/Resolucion/TABME_V1.0_2017.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB-USR-AQ265-A0805\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB-USR-AQ265-A0106\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Tableros" sheetId="1" r:id="rId1"/>
@@ -1480,16 +1480,19 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1512,9 +1515,6 @@
     </xf>
     <xf numFmtId="1" fontId="20" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1677,7 +1677,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1742,11 +1741,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="201240384"/>
-        <c:axId val="201241504"/>
+        <c:axId val="273670192"/>
+        <c:axId val="273670752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="201240384"/>
+        <c:axId val="273670192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1778,7 +1777,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1825,7 +1823,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201241504"/>
+        <c:crossAx val="273670752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1833,7 +1831,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201241504"/>
+        <c:axId val="273670752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1891,7 +1889,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1905,7 +1902,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201240384"/>
+        <c:crossAx val="273670192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2105,7 +2102,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -2168,11 +2164,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="201245984"/>
-        <c:axId val="201246544"/>
+        <c:axId val="273673552"/>
+        <c:axId val="273674112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="201245984"/>
+        <c:axId val="273673552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2215,7 +2211,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201246544"/>
+        <c:crossAx val="273674112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2223,7 +2219,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201246544"/>
+        <c:axId val="273674112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2244,7 +2240,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201245984"/>
+        <c:crossAx val="273673552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2351,6 +2347,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2442,11 +2439,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="201249344"/>
-        <c:axId val="201249904"/>
+        <c:axId val="273676912"/>
+        <c:axId val="273677472"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="201249344"/>
+        <c:axId val="273676912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,6 +2475,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2524,7 +2522,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201249904"/>
+        <c:crossAx val="273677472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2532,7 +2530,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201249904"/>
+        <c:axId val="273677472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2578,6 +2576,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2618,7 +2617,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201249344"/>
+        <c:crossAx val="273676912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2632,6 +2631,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
@@ -2874,12 +2874,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="201252144"/>
-        <c:axId val="201252704"/>
+        <c:axId val="275480912"/>
+        <c:axId val="275481472"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="201252144"/>
+        <c:axId val="275480912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2916,7 +2916,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201252704"/>
+        <c:crossAx val="275481472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2924,7 +2924,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="201252704"/>
+        <c:axId val="275481472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2972,7 +2972,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="201252144"/>
+        <c:crossAx val="275480912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3201,11 +3201,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="201255504"/>
-        <c:axId val="261730112"/>
+        <c:axId val="275484272"/>
+        <c:axId val="275484832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="201255504"/>
+        <c:axId val="275484272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3289,7 +3289,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261730112"/>
+        <c:crossAx val="275484832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3297,7 +3297,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261730112"/>
+        <c:axId val="275484832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3359,7 +3359,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="201255504"/>
+        <c:crossAx val="275484272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3581,11 +3581,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="261732352"/>
-        <c:axId val="261732912"/>
+        <c:axId val="275487072"/>
+        <c:axId val="275487632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261732352"/>
+        <c:axId val="275487072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3661,7 +3661,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261732912"/>
+        <c:crossAx val="275487632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3669,7 +3669,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261732912"/>
+        <c:axId val="275487632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3753,7 +3753,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261732352"/>
+        <c:crossAx val="275487072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3949,6 +3949,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4013,11 +4014,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="261735712"/>
-        <c:axId val="261736272"/>
+        <c:axId val="275490432"/>
+        <c:axId val="275490992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="261735712"/>
+        <c:axId val="275490432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4049,6 +4050,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4095,7 +4097,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261736272"/>
+        <c:crossAx val="275490992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4103,7 +4105,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261736272"/>
+        <c:axId val="275490992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4166,6 +4168,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4179,7 +4182,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261735712"/>
+        <c:crossAx val="275490432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4379,6 +4382,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -4441,11 +4445,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="65"/>
-        <c:axId val="261738512"/>
-        <c:axId val="261739072"/>
+        <c:axId val="275493232"/>
+        <c:axId val="275493792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261738512"/>
+        <c:axId val="275493232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4488,7 +4492,7 @@
             <a:endParaRPr lang="es-PE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261739072"/>
+        <c:crossAx val="275493792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4496,7 +4500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261739072"/>
+        <c:axId val="275493792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4517,7 +4521,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261738512"/>
+        <c:crossAx val="275493232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6062,7 +6066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
@@ -6721,8 +6725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+    <sheetView topLeftCell="A22" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6888,7 +6892,7 @@
       <c r="F15" s="134"/>
       <c r="G15" s="134"/>
       <c r="H15" s="134"/>
-      <c r="I15" s="153"/>
+      <c r="I15" s="156"/>
       <c r="J15" s="95"/>
     </row>
     <row r="16" spans="1:12" ht="30.75" customHeight="1" thickBot="1">
@@ -7009,7 +7013,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G23" s="68">
         <f>E23/F23</f>
@@ -7076,7 +7080,7 @@
         <v>0</v>
       </c>
       <c r="F29" s="44">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G29" s="67">
         <f>E29/F29*100</f>
@@ -7098,14 +7102,14 @@
       <c r="H30" s="74"/>
     </row>
     <row r="31" spans="1:9" ht="18.75">
-      <c r="A31" s="156"/>
-      <c r="B31" s="156"/>
-      <c r="C31" s="156"/>
-      <c r="D31" s="156"/>
-      <c r="E31" s="156"/>
-      <c r="F31" s="156"/>
-      <c r="G31" s="156"/>
-      <c r="H31" s="156"/>
+      <c r="A31" s="155"/>
+      <c r="B31" s="155"/>
+      <c r="C31" s="155"/>
+      <c r="D31" s="155"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="155"/>
+      <c r="G31" s="155"/>
+      <c r="H31" s="155"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="49"/>
@@ -7137,7 +7141,7 @@
       <c r="D39" s="134"/>
       <c r="E39" s="134"/>
       <c r="F39" s="134"/>
-      <c r="G39" s="153"/>
+      <c r="G39" s="156"/>
       <c r="H39" s="95"/>
     </row>
     <row r="40" spans="1:8" ht="24.75" thickBot="1">
@@ -7185,10 +7189,10 @@
       <c r="B42" s="144"/>
       <c r="C42" s="144"/>
       <c r="D42" s="20">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E42" s="89">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F42" s="53" t="s">
         <v>36</v>
@@ -7222,10 +7226,10 @@
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="46" spans="1:8" ht="50.25" customHeight="1">
-      <c r="A46" s="154" t="s">
+      <c r="A46" s="153" t="s">
         <v>38</v>
       </c>
-      <c r="B46" s="155"/>
+      <c r="B46" s="154"/>
     </row>
     <row r="47" spans="1:8" ht="15.75">
       <c r="A47" s="22" t="s">
@@ -7397,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -7538,15 +7542,15 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A15" s="157" t="s">
+      <c r="A15" s="158" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="158"/>
-      <c r="C15" s="158"/>
-      <c r="D15" s="158"/>
-      <c r="E15" s="158"/>
-      <c r="F15" s="158"/>
-      <c r="G15" s="158"/>
+      <c r="B15" s="159"/>
+      <c r="C15" s="159"/>
+      <c r="D15" s="159"/>
+      <c r="E15" s="159"/>
+      <c r="F15" s="159"/>
+      <c r="G15" s="159"/>
     </row>
     <row r="16" spans="1:10" ht="36.75" thickBot="1">
       <c r="A16" s="36" t="s">
@@ -7597,15 +7601,15 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.5" customHeight="1" thickBot="1">
-      <c r="A22" s="160" t="s">
+      <c r="A22" s="161" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="161"/>
-      <c r="C22" s="161"/>
-      <c r="D22" s="161"/>
-      <c r="E22" s="161"/>
-      <c r="F22" s="161"/>
-      <c r="G22" s="161"/>
+      <c r="B22" s="162"/>
+      <c r="C22" s="162"/>
+      <c r="D22" s="162"/>
+      <c r="E22" s="162"/>
+      <c r="F22" s="162"/>
+      <c r="G22" s="162"/>
     </row>
     <row r="23" spans="1:7" ht="36.75" thickBot="1">
       <c r="A23" s="36" t="s">
@@ -7680,15 +7684,15 @@
       <c r="F29" s="86"/>
     </row>
     <row r="34" spans="1:14" ht="19.5" customHeight="1">
-      <c r="A34" s="159" t="s">
+      <c r="A34" s="160" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="159"/>
-      <c r="C34" s="159"/>
-      <c r="D34" s="159"/>
-      <c r="E34" s="159"/>
-      <c r="F34" s="159"/>
-      <c r="G34" s="159"/>
+      <c r="B34" s="160"/>
+      <c r="C34" s="160"/>
+      <c r="D34" s="160"/>
+      <c r="E34" s="160"/>
+      <c r="F34" s="160"/>
+      <c r="G34" s="160"/>
       <c r="H34" s="95"/>
       <c r="L34" s="64"/>
       <c r="M34" s="65"/>
@@ -7710,8 +7714,8 @@
       <c r="E35" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="F35" s="164"/>
-      <c r="G35" s="164"/>
+      <c r="F35" s="157"/>
+      <c r="G35" s="157"/>
       <c r="K35" s="64"/>
       <c r="L35" s="65"/>
       <c r="M35" s="65"/>
@@ -7732,22 +7736,22 @@
       <c r="E36" s="80">
         <v>26</v>
       </c>
-      <c r="F36" s="164"/>
-      <c r="G36" s="164"/>
+      <c r="F36" s="157"/>
+      <c r="G36" s="157"/>
       <c r="K36" s="64"/>
       <c r="L36" s="65"/>
       <c r="M36" s="65"/>
     </row>
     <row r="37" spans="1:14" ht="26.25" customHeight="1">
-      <c r="A37" s="162" t="s">
+      <c r="A37" s="163" t="s">
         <v>43</v>
       </c>
-      <c r="B37" s="162"/>
-      <c r="C37" s="162"/>
-      <c r="D37" s="163">
+      <c r="B37" s="163"/>
+      <c r="C37" s="163"/>
+      <c r="D37" s="164">
         <v>26</v>
       </c>
-      <c r="E37" s="163">
+      <c r="E37" s="164">
         <v>26</v>
       </c>
       <c r="F37" s="97" t="s">
@@ -7758,11 +7762,11 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="162"/>
-      <c r="B38" s="162"/>
-      <c r="C38" s="162"/>
-      <c r="D38" s="163"/>
-      <c r="E38" s="163"/>
+      <c r="A38" s="163"/>
+      <c r="B38" s="163"/>
+      <c r="C38" s="163"/>
+      <c r="D38" s="164"/>
+      <c r="E38" s="164"/>
       <c r="F38" s="63">
         <f>+G38</f>
         <v>26</v>
@@ -7908,8 +7912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U42"/>
   <sheetViews>
-    <sheetView topLeftCell="B32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q38" sqref="Q38"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8113,16 +8117,16 @@
       </c>
     </row>
     <row r="15" spans="1:19" ht="32.25" customHeight="1">
-      <c r="A15" s="159" t="s">
+      <c r="A15" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="159"/>
-      <c r="C15" s="159"/>
-      <c r="D15" s="159"/>
-      <c r="E15" s="159"/>
-      <c r="F15" s="159"/>
-      <c r="G15" s="159"/>
-      <c r="H15" s="159"/>
+      <c r="B15" s="160"/>
+      <c r="C15" s="160"/>
+      <c r="D15" s="160"/>
+      <c r="E15" s="160"/>
+      <c r="F15" s="160"/>
+      <c r="G15" s="160"/>
+      <c r="H15" s="160"/>
       <c r="I15" s="95"/>
       <c r="J15" s="47"/>
       <c r="K15" s="47"/>
@@ -8182,16 +8186,16 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="30.75" customHeight="1">
-      <c r="A20" s="159" t="s">
+      <c r="A20" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="159"/>
-      <c r="C20" s="159"/>
-      <c r="D20" s="159"/>
-      <c r="E20" s="159"/>
-      <c r="F20" s="159"/>
-      <c r="G20" s="159"/>
-      <c r="H20" s="159"/>
+      <c r="B20" s="160"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="160"/>
+      <c r="H20" s="160"/>
       <c r="I20" s="95"/>
     </row>
     <row r="21" spans="1:11" ht="48.75" customHeight="1">
@@ -8237,7 +8241,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="79">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G22" s="35">
         <f>E22/F22</f>
@@ -8304,15 +8308,15 @@
       <c r="I27" s="74"/>
     </row>
     <row r="29" spans="1:11" ht="42.75" customHeight="1">
-      <c r="A29" s="159" t="s">
+      <c r="A29" s="160" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="159"/>
-      <c r="C29" s="159"/>
-      <c r="D29" s="159"/>
-      <c r="E29" s="159"/>
-      <c r="F29" s="159"/>
-      <c r="G29" s="159"/>
+      <c r="B29" s="160"/>
+      <c r="C29" s="160"/>
+      <c r="D29" s="160"/>
+      <c r="E29" s="160"/>
+      <c r="F29" s="160"/>
+      <c r="G29" s="160"/>
       <c r="H29" s="95"/>
       <c r="I29" s="95"/>
       <c r="J29" s="47"/>
@@ -8334,8 +8338,8 @@
       <c r="E30" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="F30" s="164"/>
-      <c r="G30" s="164"/>
+      <c r="F30" s="157"/>
+      <c r="G30" s="157"/>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
     </row>
@@ -8355,8 +8359,8 @@
       <c r="E31" s="79">
         <v>0</v>
       </c>
-      <c r="F31" s="164"/>
-      <c r="G31" s="164"/>
+      <c r="F31" s="157"/>
+      <c r="G31" s="157"/>
       <c r="H31" s="50"/>
       <c r="I31" s="51"/>
     </row>
@@ -8370,7 +8374,7 @@
         <v>22</v>
       </c>
       <c r="E32" s="79">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F32" s="97" t="s">
         <v>36</v>

</xml_diff>